<commit_message>
New attributes for user and assignment
</commit_message>
<xml_diff>
--- a/papers/attributes.xlsx
+++ b/papers/attributes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F97E621E-2C79-4C65-B6D4-EBF319848EB1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D4E7C36A-CE60-42B6-A576-805E159034D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>assignment</t>
   </si>
@@ -37,19 +37,49 @@
     <t>user</t>
   </si>
   <si>
-    <t>student/working</t>
-  </si>
-  <si>
     <t>marital status</t>
   </si>
   <si>
-    <t>job/intern/learning</t>
-  </si>
-  <si>
     <t>travel_time</t>
   </si>
   <si>
     <t>internet_at_home</t>
+  </si>
+  <si>
+    <t>branch_of_study</t>
+  </si>
+  <si>
+    <t>math/non_math</t>
+  </si>
+  <si>
+    <t>working/non-working</t>
+  </si>
+  <si>
+    <t>total_login_time</t>
+  </si>
+  <si>
+    <t>total_classes_attended</t>
+  </si>
+  <si>
+    <t>total_assignments_completed</t>
+  </si>
+  <si>
+    <t>free_time_after_college</t>
+  </si>
+  <si>
+    <t>error_count</t>
+  </si>
+  <si>
+    <t>times_executed</t>
+  </si>
+  <si>
+    <t>time_taken_to_solve</t>
+  </si>
+  <si>
+    <t>keystrokes (backspace)</t>
+  </si>
+  <si>
+    <t>job/intern/learning/corporate</t>
   </si>
 </sst>
 </file>
@@ -376,16 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -400,40 +430,87 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>